<commit_message>
able to start community games
Signed-off-by: Gian Federspiel <gian.federspiel@bluewin.ch>
</commit_message>
<xml_diff>
--- a/Documents/Zeitplanung.xlsx
+++ b/Documents/Zeitplanung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Fancy_BLJ-Gamelauncher\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F839EDAA-7CA7-4DB7-B76E-C43730F0C0CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8C1B2F-144A-4DDF-9CC9-4B35847F022F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2295" windowWidth="29040" windowHeight="15840" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1830" windowWidth="29040" windowHeight="17640" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplanung" sheetId="1" r:id="rId1"/>
@@ -1668,7 +1668,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2175,8 +2175,8 @@
   </sheetPr>
   <dimension ref="A1:BJ47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="Y13" sqref="Y13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AC29" sqref="AC29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -3446,7 +3446,7 @@
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D34)</f>
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -4346,7 +4346,7 @@
       </c>
       <c r="D30" s="82">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E30" s="50"/>
       <c r="F30" s="51"/>
@@ -4368,7 +4368,9 @@
       <c r="T30" s="58"/>
       <c r="U30" s="59"/>
       <c r="V30" s="60"/>
-      <c r="W30" s="55"/>
+      <c r="W30" s="55">
+        <v>2</v>
+      </c>
       <c r="X30" s="92"/>
       <c r="Y30" s="56"/>
       <c r="Z30" s="57"/>
@@ -4414,14 +4416,14 @@
         <v>313</v>
       </c>
       <c r="B31" s="46" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C31" s="49">
         <v>4</v>
       </c>
       <c r="D31" s="82">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E31" s="50"/>
       <c r="F31" s="51"/>
@@ -4441,9 +4443,15 @@
       <c r="T31" s="58"/>
       <c r="U31" s="59"/>
       <c r="V31" s="60"/>
-      <c r="W31" s="55"/>
-      <c r="X31" s="93"/>
-      <c r="Y31" s="92"/>
+      <c r="W31" s="55">
+        <v>4</v>
+      </c>
+      <c r="X31" s="93">
+        <v>8</v>
+      </c>
+      <c r="Y31" s="92">
+        <v>2</v>
+      </c>
       <c r="Z31" s="57"/>
       <c r="AA31" s="58"/>
       <c r="AB31" s="61"/>
@@ -4487,14 +4495,14 @@
         <v>314</v>
       </c>
       <c r="B32" s="46" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C32" s="49">
         <v>4</v>
       </c>
       <c r="D32" s="82">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E32" s="50"/>
       <c r="F32" s="51"/>
@@ -4514,7 +4522,9 @@
       <c r="T32" s="58"/>
       <c r="U32" s="59"/>
       <c r="V32" s="60"/>
-      <c r="W32" s="55"/>
+      <c r="W32" s="55">
+        <v>2</v>
+      </c>
       <c r="X32" s="55"/>
       <c r="Y32" s="92"/>
       <c r="Z32" s="57"/>
@@ -4567,7 +4577,7 @@
       </c>
       <c r="D33" s="82">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E33" s="50"/>
       <c r="F33" s="51"/>
@@ -4589,7 +4599,9 @@
       <c r="V33" s="71"/>
       <c r="W33" s="55"/>
       <c r="X33" s="55"/>
-      <c r="Y33" s="56"/>
+      <c r="Y33" s="56">
+        <v>2</v>
+      </c>
       <c r="Z33" s="57"/>
       <c r="AA33" s="58"/>
       <c r="AB33" s="95"/>
@@ -4640,7 +4652,7 @@
       </c>
       <c r="D34" s="82">
         <f>SUM(G34:BJ34)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E34" s="50"/>
       <c r="F34" s="51"/>
@@ -4662,7 +4674,9 @@
       <c r="V34" s="71"/>
       <c r="W34" s="55"/>
       <c r="X34" s="55"/>
-      <c r="Y34" s="56"/>
+      <c r="Y34" s="56">
+        <v>4</v>
+      </c>
       <c r="Z34" s="57"/>
       <c r="AA34" s="58"/>
       <c r="AB34" s="95"/>
@@ -5579,7 +5593,7 @@
       </c>
       <c r="D47" s="37">
         <f>D43+D40+D35+D18+D14+D9</f>
-        <v>35.299999999999997</v>
+        <v>59.3</v>
       </c>
       <c r="E47" s="37"/>
       <c r="F47" s="38"/>
@@ -5649,15 +5663,15 @@
       </c>
       <c r="W47" s="39">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="X47" s="39">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Y47" s="39">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Z47" s="39">
         <f t="shared" si="4"/>
@@ -5911,7 +5925,7 @@
       </c>
       <c r="D5" s="79">
         <f>Zeitplanung!D18</f>
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="E5" s="81"/>
       <c r="F5" s="80"/>

</xml_diff>